<commit_message>
commit para hacer el pull y bajar lo ultimo de GestionDocumental Irina
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Cotización AP No Enlatada.xlsx
+++ b/Sura/DataSource - Cotización AP No Enlatada.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFA299C-4062-49A4-9B9D-86DC2CCFBC65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD87F20-0ED7-443D-B955-DDEF353FFE9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Usuario</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Cupón</t>
+  </si>
+  <si>
+    <t>https://i-preproducciongestion.segurossura.com.ar/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>i-preproducciongestion.segurossura.com.ar</t>
   </si>
 </sst>
 </file>
@@ -549,12 +555,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
@@ -630,10 +637,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -642,7 +649,7 @@
         <v>28</v>
       </c>
       <c r="E2">
-        <v>7557632631</v>
+        <v>2240451788</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>

</xml_diff>